<commit_message>
Auto-committed on 2023/02/16 週四 17:40:17.08
</commit_message>
<xml_diff>
--- a/Program/Other/LY005_底稿_非RBC_表20_會計部年度檢查報表.xlsx
+++ b/Program/Other/LY005_底稿_非RBC_表20_會計部年度檢查報表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF30DD1-F6E2-4F10-85B1-27D6921DE0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AD0A3E-CE68-4BC2-9926-54FC3FEAB50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YYY.MM" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">YYY.MM!$B$1:$P$18</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">YYY.MM!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="181029" refMode="R1C1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -823,168 +814,150 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="57" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="57" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="57" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="57" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="11"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="11"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="11" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1406,62 +1379,57 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" style="38" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" style="26" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="38" customWidth="1"/>
-    <col min="6" max="7" width="4.109375" style="38" customWidth="1"/>
-    <col min="8" max="8" width="66.33203125" style="38" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="28" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="38" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" style="38" customWidth="1"/>
-    <col min="12" max="12" width="4.77734375" style="38" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" style="38" customWidth="1"/>
-    <col min="14" max="15" width="7.88671875" style="38" customWidth="1"/>
-    <col min="16" max="16" width="10.109375" style="38" customWidth="1"/>
-    <col min="17" max="17" width="19.44140625" style="38" customWidth="1"/>
-    <col min="18" max="18" width="17.77734375" style="39" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="7.88671875" style="38"/>
+    <col min="2" max="2" width="5.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="4.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="66.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4.77734375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" style="2" customWidth="1"/>
+    <col min="14" max="15" width="7.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="19.44140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="7.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:18">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="I1" s="4"/>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41" t="s">
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="41"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="32" t="s">
-        <v>36</v>
-      </c>
+      <c r="O1" s="47"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="28"/>
     </row>
     <row r="2" spans="1:18" s="8" customFormat="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="7"/>
       <c r="F2" s="6"/>
       <c r="G2" s="2"/>
@@ -1471,19 +1439,19 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="42" t="s">
+      <c r="N2" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="32" t="s">
-        <v>35</v>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="28" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" ht="81">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45" t="s">
+    <row r="3" spans="1:18" ht="81">
+      <c r="A3" s="43"/>
+      <c r="B3" s="44" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1528,11 +1496,13 @@
       <c r="P3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="6"/>
+      <c r="R3" s="28" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
+    <row r="4" spans="1:18">
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="14" t="s">
         <v>17</v>
       </c>
@@ -1576,9 +1546,8 @@
         <v>30</v>
       </c>
       <c r="Q4" s="5"/>
-      <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:18" s="2" customFormat="1">
+    <row r="5" spans="1:18">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="18"/>
@@ -1588,288 +1557,290 @@
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="53"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="37"/>
       <c r="O5" s="20"/>
       <c r="P5" s="23"/>
-      <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18" s="2" customFormat="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26" t="s">
+    <row r="6" spans="1:18">
+      <c r="B6" s="5"/>
+      <c r="D6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="25"/>
-      <c r="R6" s="6"/>
+      <c r="H6" s="24"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="24"/>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="24"/>
-      <c r="B9" s="33" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="24"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="24"/>
-      <c r="B11" s="33" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="24"/>
-      <c r="B12" s="33" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="24"/>
-      <c r="B13" s="33" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="24"/>
-      <c r="B14" s="33" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="24"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="24"/>
-      <c r="B16" s="33" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="24"/>
-      <c r="B17" s="33" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="34" t="s">
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="48" t="s">
+      <c r="I18" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="38" t="s">
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O18" s="31"/>
+      <c r="O18" s="27"/>
     </row>
   </sheetData>
   <autoFilter ref="C4:P18" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="19">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="C11:P11"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C8:P8"/>
+    <mergeCell ref="C9:P9"/>
+    <mergeCell ref="C10:P10"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="C12:P12"/>
@@ -1878,17 +1849,6 @@
     <mergeCell ref="C15:P15"/>
     <mergeCell ref="C16:P16"/>
     <mergeCell ref="C17:P17"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C8:P8"/>
-    <mergeCell ref="C9:P9"/>
-    <mergeCell ref="C10:P10"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="C11:P11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>